<commit_message>
Start position get tested
</commit_message>
<xml_diff>
--- a/Docs/MainScreen.xlsx
+++ b/Docs/MainScreen.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\artic\poolChess\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF88BDF-9B28-4F54-90AF-7097A9AF12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="10320" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1050" windowWidth="10320" windowHeight="10575"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -93,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,17 +468,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL11" sqref="AL11"/>
+      <selection pane="bottomRight" activeCell="AS25" sqref="AS25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="24" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="24" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="9" customWidth="1"/>
     <col min="2" max="65" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
@@ -2557,63 +2556,62 @@
       <c r="AL24" s="11">
         <v>2</v>
       </c>
-      <c r="AM24" s="2" t="s">
+      <c r="AN24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AN24" s="2" t="s">
+      <c r="AO24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AO24" s="2" t="s">
+      <c r="AP24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AP24" s="2" t="s">
+      <c r="AQ24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AQ24" s="2" t="s">
+      <c r="AR24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AR24" s="2"/>
-      <c r="AS24" s="2" t="s">
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AT24" s="2" t="s">
+      <c r="AU24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AU24" s="2" t="s">
+      <c r="AV24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AV24" s="2" t="s">
+      <c r="AW24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AW24" s="2" t="s">
+      <c r="AX24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AX24" s="2"/>
-      <c r="AY24" s="2" t="s">
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AZ24" s="2" t="s">
+      <c r="BA24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="BA24" s="2" t="s">
+      <c r="BB24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BB24" s="2" t="s">
+      <c r="BC24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="BC24" s="2" t="s">
+      <c r="BD24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="BD24" s="2" t="s">
+      <c r="BE24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="BE24" s="2" t="s">
+      <c r="BF24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="BF24" s="2" t="s">
+      <c r="BG24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="BG24" s="2"/>
       <c r="BH24" s="2"/>
       <c r="BI24" s="2"/>
       <c r="BJ24" s="2"/>
@@ -2664,7 +2662,6 @@
       <c r="AL25" s="11">
         <v>3</v>
       </c>
-      <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
       <c r="AP25" s="2"/>
@@ -2735,9 +2732,8 @@
       <c r="AL26" s="11">
         <v>4</v>
       </c>
-      <c r="AM26" s="10"/>
       <c r="AN26" s="10"/>
-      <c r="BG26" s="2"/>
+      <c r="AO26" s="10"/>
       <c r="BH26" s="2"/>
       <c r="BI26" s="2"/>
       <c r="BJ26" s="2"/>

</xml_diff>